<commit_message>
Fixed issue in python script. Was trying to sort a list and compare to an unordered dict so valid neighbors was never going to work. Changed to ordered dict so now neighbors are accurate. First few collapses still had minor issues
</commit_message>
<xml_diff>
--- a/Required_Pieces.xlsx
+++ b/Required_Pieces.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\Projects\EtG Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C42FEF-1C26-466E-B238-4BA19C3B219D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4439997C-2DFB-45DD-8CA5-A77BB6C947D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D593FF75-6177-4E51-8B01-D01C3053B7A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D593FF75-6177-4E51-8B01-D01C3053B7A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Permutations" sheetId="1" r:id="rId1"/>
     <sheet name="Unique Shapes (Expanded)" sheetId="2" r:id="rId2"/>
+    <sheet name="Inactive Neighbors Check" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="79">
   <si>
     <t>x</t>
   </si>
@@ -215,6 +216,54 @@
   </si>
   <si>
     <t>Note: walls bordering the 3 inactive areas, but still has some room for player to move around in</t>
+  </si>
+  <si>
+    <t>5_f</t>
+  </si>
+  <si>
+    <t>9_f</t>
+  </si>
+  <si>
+    <t>13_f</t>
+  </si>
+  <si>
+    <t>15_f</t>
+  </si>
+  <si>
+    <t>19_f</t>
+  </si>
+  <si>
+    <t>21_f</t>
+  </si>
+  <si>
+    <t>24_f</t>
+  </si>
+  <si>
+    <t>27_f</t>
+  </si>
+  <si>
+    <t>14_f</t>
+  </si>
+  <si>
+    <t>20_f</t>
+  </si>
+  <si>
+    <t>23_f</t>
+  </si>
+  <si>
+    <t>28_f</t>
+  </si>
+  <si>
+    <t>7_f</t>
+  </si>
+  <si>
+    <t>North Exp</t>
+  </si>
+  <si>
+    <t>North Act</t>
+  </si>
+  <si>
+    <t>11 14 14_f have top row blocked</t>
   </si>
 </sst>
 </file>
@@ -243,7 +292,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +341,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -320,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -359,6 +414,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,12 +736,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF49452-D2E7-48B4-B56B-3032190D1445}">
   <dimension ref="A2:AG232"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="3" max="28" width="6.140625" style="4" customWidth="1"/>
     <col min="29" max="29" width="5.7109375" style="4" customWidth="1"/>
     <col min="30" max="33" width="5.7109375" customWidth="1"/>
@@ -3763,8 +3825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4EB20AA-5C79-4234-B340-A0FA8AFD9F51}">
   <dimension ref="A1:P227"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P231" sqref="P231"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6289,4 +6351,195 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE07C483-88AD-4EA6-B8B7-8DEF21CEBA07}">
+  <dimension ref="B2:T11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="19" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="4">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="4">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="4">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="4">
+        <v>15</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="4">
+        <v>19</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="4">
+        <v>21</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="4">
+        <v>24</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>27</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="S2" s="4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="22">
+        <v>11</v>
+      </c>
+      <c r="D4" s="22">
+        <v>14</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="4">
+        <v>15</v>
+      </c>
+      <c r="G4" s="22">
+        <v>16</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="22">
+        <v>23</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" s="4">
+        <v>24</v>
+      </c>
+      <c r="M4" s="22">
+        <v>25</v>
+      </c>
+      <c r="N4" s="4">
+        <v>27</v>
+      </c>
+      <c r="O4" s="4">
+        <v>28</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q4" s="22">
+        <v>3</v>
+      </c>
+      <c r="R4" s="22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C7" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="23">
+        <v>13</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="23">
+        <v>15</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="23">
+        <v>19</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" s="23">
+        <v>21</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="K11" s="23">
+        <v>24</v>
+      </c>
+      <c r="L11" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" s="23">
+        <v>27</v>
+      </c>
+      <c r="N11" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="O11" s="23">
+        <v>28</v>
+      </c>
+      <c r="P11" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q11" s="23">
+        <v>5</v>
+      </c>
+      <c r="R11" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="S11" s="23">
+        <v>9</v>
+      </c>
+      <c r="T11" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>